<commit_message>
Here is the message for the Test 1234
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilding\Documents\GIT_Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E37CA8-C842-41A8-9F2B-23AE1CD5D212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD200C50-4517-4CAC-ADCE-F41E59D94E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-4446" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,6 +376,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes to .txt and .xlsx
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilding\Documents\GIT_Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD200C50-4517-4CAC-ADCE-F41E59D94E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D353E0C6-F545-4060-8550-F4F607F337E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-4446" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,6 +390,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>